<commit_message>
Updated feature files and Login changes
</commit_message>
<xml_diff>
--- a/src/test/resources/excel_files/ZainGroup_MenuListOrder.xlsx
+++ b/src/test/resources/excel_files/ZainGroup_MenuListOrder.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B101A107-CB51-4D18-BA7A-5847DE05CDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dawood.Ibrahim.EUROLAND\IdeaProjects\IRAPPV3_Automation\src\test\resources\excel_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B842C7-9850-4580-9E05-8E329AACFC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,9 +80,6 @@
     <t>Investment Calculator</t>
   </si>
   <si>
-    <t>Dividends</t>
-  </si>
-  <si>
     <t>Financial Calendar</t>
   </si>
   <si>
@@ -91,13 +93,16 @@
   </si>
   <si>
     <t>Settings</t>
+  </si>
+  <si>
+    <t>Dividend</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,33 +486,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="2" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -515,32 +520,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -548,49 +553,49 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -602,6 +607,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebebba1-b7b4-4361-ae8e-c06f2839feac">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="43182e7f-f818-4f03-9fbf-08e6341aa70f" xsi:nil="true"/>
+    <Dateandtime xmlns="eebebba1-b7b4-4361-ae8e-c06f2839feac" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A17BA758DAF1B4AB70B9D3AD1E1465C" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bf388b1aba45cd0dcf502d46e33902a1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eebebba1-b7b4-4361-ae8e-c06f2839feac" xmlns:ns3="43182e7f-f818-4f03-9fbf-08e6341aa70f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e0680d011e54198a97404d3a479e95f8" ns2:_="" ns3:_="">
     <xsd:import namespace="eebebba1-b7b4-4361-ae8e-c06f2839feac"/>
@@ -862,35 +888,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D055BD2E-F1DB-40E5-8F8B-77965196CDAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="eebebba1-b7b4-4361-ae8e-c06f2839feac"/>
+    <ds:schemaRef ds:uri="43182e7f-f818-4f03-9fbf-08e6341aa70f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebebba1-b7b4-4361-ae8e-c06f2839feac">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="43182e7f-f818-4f03-9fbf-08e6341aa70f" xsi:nil="true"/>
-    <Dateandtime xmlns="eebebba1-b7b4-4361-ae8e-c06f2839feac" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6096E87B-3229-4F74-BAB5-7E03425EBF41}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A482F97D-E695-4716-8F10-3D544D0D4CD4}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6096E87B-3229-4F74-BAB5-7E03425EBF41}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D055BD2E-F1DB-40E5-8F8B-77965196CDAB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A482F97D-E695-4716-8F10-3D544D0D4CD4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="eebebba1-b7b4-4361-ae8e-c06f2839feac"/>
+    <ds:schemaRef ds:uri="43182e7f-f818-4f03-9fbf-08e6341aa70f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>